<commit_message>
Thu Mar  2 15:22:07 EST 2017
</commit_message>
<xml_diff>
--- a/dat/map.xlsx
+++ b/dat/map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\588648\workspace\FFBase\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\588648\workspace\FFBase\dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ROOM 1</t>
   </si>
   <si>
     <t>ROOM 12</t>
+  </si>
+  <si>
+    <t>ROOM 139</t>
+  </si>
+  <si>
+    <t>ROOM 71</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,6 +216,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,27 +501,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="XP1334:YF1341"/>
+  <dimension ref="XL1334:YF1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="XK1320" workbookViewId="0">
-      <selection activeCell="YB1322" sqref="YB1322"/>
+    <sheetView tabSelected="1" topLeftCell="XK1323" workbookViewId="0">
+      <selection activeCell="YB1331" sqref="YB1331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="641" width="8.88671875" style="1"/>
-    <col min="642" max="642" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="643" max="646" width="8.88671875" style="1"/>
-    <col min="647" max="647" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="648" max="1260" width="8.88671875" style="1"/>
+    <col min="1" max="636" width="8.88671875" style="1"/>
+    <col min="637" max="637" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="638" max="639" width="8.88671875" style="1"/>
+    <col min="640" max="646" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="647" max="647" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="648" max="652" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="653" max="653" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="654" max="656" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="657" max="1260" width="8.88671875" style="1"/>
     <col min="1261" max="1261" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="1262" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1334" spans="640:656" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="1335" spans="640:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1334" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1335" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XZ1335" s="7" t="str">
-        <f t="shared" ref="XP1335:YF1341" ca="1" si="0">CONCATENATE(CELL("col",XZ1335)-1,",",CELL("row",XZ1335)-1)</f>
+        <f t="shared" ref="XL1335:YF1341" ca="1" si="0">CONCATENATE(CELL("col",XZ1335)-1,",",CELL("row",XZ1335)-1)</f>
         <v>649,1334</v>
       </c>
       <c r="YA1335" s="8" t="str">
@@ -540,7 +553,19 @@
         <v>655,1334</v>
       </c>
     </row>
-    <row r="1336" spans="640:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1336" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XL1336" s="7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1335</v>
+      </c>
+      <c r="XM1336" s="16" t="str">
+        <f t="shared" ref="XM1336:XM1338" ca="1" si="1">CONCATENATE(CELL("col",XM1336)-1,",",CELL("row",XM1336)-1)</f>
+        <v>636,1335</v>
+      </c>
+      <c r="XN1336" s="9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>637,1335</v>
+      </c>
       <c r="XP1336" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1335</v>
@@ -590,7 +615,23 @@
         <v>655,1335</v>
       </c>
     </row>
-    <row r="1337" spans="640:656" x14ac:dyDescent="0.3">
+    <row r="1337" spans="636:656" x14ac:dyDescent="0.3">
+      <c r="XL1337" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1336</v>
+      </c>
+      <c r="XM1337" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>636,1336</v>
+      </c>
+      <c r="XN1337" s="12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>637,1336</v>
+      </c>
+      <c r="XO1337" s="9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>638,1336</v>
+      </c>
       <c r="XP1337" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1336</v>
@@ -660,7 +701,22 @@
         <v>655,1336</v>
       </c>
     </row>
-    <row r="1338" spans="640:656" x14ac:dyDescent="0.3">
+    <row r="1338" spans="636:656" x14ac:dyDescent="0.3">
+      <c r="XL1338" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1337</v>
+      </c>
+      <c r="XM1338" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="XN1338" s="3" t="str">
+        <f t="shared" ref="XN1338:XN1339" ca="1" si="2">CONCATENATE(CELL("col",XN1338)-1,",",CELL("row",XN1338)-1)</f>
+        <v>637,1337</v>
+      </c>
+      <c r="XO1338" s="4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>638,1337</v>
+      </c>
       <c r="XP1338" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1337</v>
@@ -699,7 +755,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>648,1337</v>
       </c>
-      <c r="XZ1338" s="10" t="str">
+      <c r="XZ1338" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>649,1337</v>
       </c>
@@ -711,9 +767,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>651,1337</v>
       </c>
-      <c r="YC1338" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>652,1337</v>
+      <c r="YC1338" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="YD1338" s="12" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -728,21 +783,37 @@
         <v>655,1337</v>
       </c>
     </row>
-    <row r="1339" spans="640:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1339" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XL1339" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1338</v>
+      </c>
+      <c r="XM1339" s="3" t="str">
+        <f t="shared" ref="XM1338:XM1339" ca="1" si="3">CONCATENATE(CELL("col",XM1339)-1,",",CELL("row",XM1339)-1)</f>
+        <v>636,1338</v>
+      </c>
+      <c r="XN1339" s="3" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>637,1338</v>
+      </c>
+      <c r="XO1339" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>638,1338</v>
+      </c>
       <c r="XP1339" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1338</v>
       </c>
       <c r="XQ1339" s="3" t="str">
-        <f t="shared" ref="XQ1339:XS1340" ca="1" si="1">CONCATENATE(CELL("col",XQ1339)-1,",",CELL("row",XQ1339)-1)</f>
+        <f t="shared" ref="XQ1339:XS1340" ca="1" si="4">CONCATENATE(CELL("col",XQ1339)-1,",",CELL("row",XQ1339)-1)</f>
         <v>640,1338</v>
       </c>
       <c r="XR1339" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>641,1338</v>
       </c>
       <c r="XS1339" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>642,1338</v>
       </c>
       <c r="XT1339" s="14" t="str">
@@ -798,7 +869,23 @@
         <v>655,1338</v>
       </c>
     </row>
-    <row r="1340" spans="640:656" x14ac:dyDescent="0.3">
+    <row r="1340" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XL1340" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1339</v>
+      </c>
+      <c r="XM1340" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>636,1339</v>
+      </c>
+      <c r="XN1340" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>637,1339</v>
+      </c>
+      <c r="XO1340" s="15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>638,1339</v>
+      </c>
       <c r="XP1340" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1339</v>
@@ -808,11 +895,11 @@
         <v>640,1339</v>
       </c>
       <c r="XR1340" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>641,1339</v>
       </c>
       <c r="XS1340" s="12" t="str">
-        <f t="shared" ref="XS1340:XS1341" ca="1" si="2">CONCATENATE(CELL("col",XS1340)-1,",",CELL("row",XS1340)-1)</f>
+        <f t="shared" ref="XS1340:XS1341" ca="1" si="5">CONCATENATE(CELL("col",XS1340)-1,",",CELL("row",XS1340)-1)</f>
         <v>642,1339</v>
       </c>
       <c r="XT1340" s="14" t="str">
@@ -848,7 +935,7 @@
         <v>655,1339</v>
       </c>
     </row>
-    <row r="1341" spans="640:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1341" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XP1341" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1340</v>
@@ -858,11 +945,11 @@
         <v>640,1340</v>
       </c>
       <c r="XR1341" s="5" t="str">
-        <f t="shared" ref="XR1341" ca="1" si="3">CONCATENATE(CELL("col",XR1341)-1,",",CELL("row",XR1341)-1)</f>
+        <f t="shared" ref="XR1341" ca="1" si="6">CONCATENATE(CELL("col",XR1341)-1,",",CELL("row",XR1341)-1)</f>
         <v>641,1340</v>
       </c>
       <c r="XS1341" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="5"/>
         <v>642,1340</v>
       </c>
       <c r="XT1341" s="15" t="str">

</xml_diff>

<commit_message>
Wed Mar  8 15:45:58 EST 2017
</commit_message>
<xml_diff>
--- a/dat/map.xlsx
+++ b/dat/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="8592"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ROOM 1</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>ROOM 71</t>
+  </si>
+  <si>
+    <t>ROOM 43</t>
+  </si>
+  <si>
+    <t>ROOM 82</t>
   </si>
 </sst>
 </file>
@@ -501,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="XL1334:YF1341"/>
+  <dimension ref="XG1330:YF1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="XK1323" workbookViewId="0">
-      <selection activeCell="YB1331" sqref="YB1331"/>
+    <sheetView tabSelected="1" topLeftCell="WZ1323" workbookViewId="0">
+      <selection activeCell="XE1324" sqref="XE1324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,10 +528,176 @@
     <col min="1262" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1334" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="1335" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1330" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1331" spans="631:656" x14ac:dyDescent="0.3">
+      <c r="XG1331" s="7" t="str">
+        <f t="shared" ref="XG1331:YF1341" ca="1" si="0">CONCATENATE(CELL("col",XG1331)-1,",",CELL("row",XG1331)-1)</f>
+        <v>630,1330</v>
+      </c>
+      <c r="XH1331" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>631,1330</v>
+      </c>
+      <c r="XI1331" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>632,1330</v>
+      </c>
+      <c r="XJ1331" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>633,1330</v>
+      </c>
+      <c r="XK1331" s="9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>634,1330</v>
+      </c>
+      <c r="XL1331" s="7" t="str">
+        <f t="shared" ref="XL1331:XL1332" ca="1" si="1">CONCATENATE(CELL("col",XL1331)-1,",",CELL("row",XL1331)-1)</f>
+        <v>635,1330</v>
+      </c>
+      <c r="XM1331" s="16" t="str">
+        <f t="shared" ref="XM1331:XN1331" ca="1" si="2">CONCATENATE(CELL("col",XM1331)-1,",",CELL("row",XM1331)-1)</f>
+        <v>636,1330</v>
+      </c>
+      <c r="XN1331" s="9" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>637,1330</v>
+      </c>
+    </row>
+    <row r="1332" spans="631:656" x14ac:dyDescent="0.3">
+      <c r="XG1332" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>630,1331</v>
+      </c>
+      <c r="XH1332" s="3" t="str">
+        <f t="shared" ref="XH1332:XJ1334" ca="1" si="3">CONCATENATE(CELL("col",XH1332)-1,",",CELL("row",XH1332)-1)</f>
+        <v>631,1331</v>
+      </c>
+      <c r="XI1332" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>632,1331</v>
+      </c>
+      <c r="XJ1332" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>633,1331</v>
+      </c>
+      <c r="XK1332" s="14" t="str">
+        <f t="shared" ref="XK1332:XN1334" ca="1" si="4">CONCATENATE(CELL("col",XK1332)-1,",",CELL("row",XK1332)-1)</f>
+        <v>634,1331</v>
+      </c>
+      <c r="XL1332" s="10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>635,1331</v>
+      </c>
+      <c r="XM1332" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>636,1331</v>
+      </c>
+      <c r="XN1332" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>637,1331</v>
+      </c>
+    </row>
+    <row r="1333" spans="631:656" x14ac:dyDescent="0.3">
+      <c r="XG1333" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>630,1332</v>
+      </c>
+      <c r="XH1333" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>631,1332</v>
+      </c>
+      <c r="XI1333" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>632,1332</v>
+      </c>
+      <c r="XJ1333" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="XK1333" s="4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>634,1332</v>
+      </c>
+      <c r="XL1333" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1332</v>
+      </c>
+      <c r="XM1333" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="XN1333" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>637,1332</v>
+      </c>
+    </row>
+    <row r="1334" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XG1334" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>630,1333</v>
+      </c>
+      <c r="XH1334" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>631,1333</v>
+      </c>
+      <c r="XI1334" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>632,1333</v>
+      </c>
+      <c r="XJ1334" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>633,1333</v>
+      </c>
+      <c r="XK1334" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>634,1333</v>
+      </c>
+      <c r="XL1334" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1333</v>
+      </c>
+      <c r="XM1334" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>636,1333</v>
+      </c>
+      <c r="XN1334" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>637,1333</v>
+      </c>
+    </row>
+    <row r="1335" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="XG1335" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>630,1334</v>
+      </c>
+      <c r="XH1335" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>631,1334</v>
+      </c>
+      <c r="XI1335" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>632,1334</v>
+      </c>
+      <c r="XJ1335" s="13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>633,1334</v>
+      </c>
+      <c r="XK1335" s="15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>634,1334</v>
+      </c>
+      <c r="XL1335" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>635,1334</v>
+      </c>
+      <c r="XM1335" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>636,1334</v>
+      </c>
+      <c r="XN1335" s="15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>637,1334</v>
+      </c>
       <c r="XZ1335" s="7" t="str">
-        <f t="shared" ref="XL1335:YF1341" ca="1" si="0">CONCATENATE(CELL("col",XZ1335)-1,",",CELL("row",XZ1335)-1)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>649,1334</v>
       </c>
       <c r="YA1335" s="8" t="str">
@@ -553,13 +725,13 @@
         <v>655,1334</v>
       </c>
     </row>
-    <row r="1336" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1336" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1336" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>635,1335</v>
       </c>
       <c r="XM1336" s="16" t="str">
-        <f t="shared" ref="XM1336:XM1338" ca="1" si="1">CONCATENATE(CELL("col",XM1336)-1,",",CELL("row",XM1336)-1)</f>
+        <f t="shared" ref="XM1336:XM1338" ca="1" si="5">CONCATENATE(CELL("col",XM1336)-1,",",CELL("row",XM1336)-1)</f>
         <v>636,1335</v>
       </c>
       <c r="XN1336" s="9" t="str">
@@ -615,13 +787,13 @@
         <v>655,1335</v>
       </c>
     </row>
-    <row r="1337" spans="636:656" x14ac:dyDescent="0.3">
+    <row r="1337" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XL1337" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>635,1336</v>
       </c>
       <c r="XM1337" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>636,1336</v>
       </c>
       <c r="XN1337" s="12" t="str">
@@ -701,7 +873,7 @@
         <v>655,1336</v>
       </c>
     </row>
-    <row r="1338" spans="636:656" x14ac:dyDescent="0.3">
+    <row r="1338" spans="631:656" x14ac:dyDescent="0.3">
       <c r="XL1338" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>635,1337</v>
@@ -710,7 +882,7 @@
         <v>3</v>
       </c>
       <c r="XN1338" s="3" t="str">
-        <f t="shared" ref="XN1338:XN1339" ca="1" si="2">CONCATENATE(CELL("col",XN1338)-1,",",CELL("row",XN1338)-1)</f>
+        <f t="shared" ref="XN1338:XN1339" ca="1" si="6">CONCATENATE(CELL("col",XN1338)-1,",",CELL("row",XN1338)-1)</f>
         <v>637,1337</v>
       </c>
       <c r="XO1338" s="4" t="str">
@@ -783,17 +955,17 @@
         <v>655,1337</v>
       </c>
     </row>
-    <row r="1339" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1339" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1339" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>635,1338</v>
       </c>
       <c r="XM1339" s="3" t="str">
-        <f t="shared" ref="XM1338:XM1339" ca="1" si="3">CONCATENATE(CELL("col",XM1339)-1,",",CELL("row",XM1339)-1)</f>
+        <f t="shared" ref="XM1338:XM1339" ca="1" si="7">CONCATENATE(CELL("col",XM1339)-1,",",CELL("row",XM1339)-1)</f>
         <v>636,1338</v>
       </c>
       <c r="XN1339" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>637,1338</v>
       </c>
       <c r="XO1339" s="14" t="str">
@@ -805,15 +977,15 @@
         <v>639,1338</v>
       </c>
       <c r="XQ1339" s="3" t="str">
-        <f t="shared" ref="XQ1339:XS1340" ca="1" si="4">CONCATENATE(CELL("col",XQ1339)-1,",",CELL("row",XQ1339)-1)</f>
+        <f t="shared" ref="XQ1339:XS1340" ca="1" si="8">CONCATENATE(CELL("col",XQ1339)-1,",",CELL("row",XQ1339)-1)</f>
         <v>640,1338</v>
       </c>
       <c r="XR1339" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>641,1338</v>
       </c>
       <c r="XS1339" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>642,1338</v>
       </c>
       <c r="XT1339" s="14" t="str">
@@ -869,7 +1041,7 @@
         <v>655,1338</v>
       </c>
     </row>
-    <row r="1340" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1340" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XL1340" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>635,1339</v>
@@ -895,11 +1067,11 @@
         <v>640,1339</v>
       </c>
       <c r="XR1340" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>641,1339</v>
       </c>
       <c r="XS1340" s="12" t="str">
-        <f t="shared" ref="XS1340:XS1341" ca="1" si="5">CONCATENATE(CELL("col",XS1340)-1,",",CELL("row",XS1340)-1)</f>
+        <f t="shared" ref="XS1340:XS1341" ca="1" si="9">CONCATENATE(CELL("col",XS1340)-1,",",CELL("row",XS1340)-1)</f>
         <v>642,1339</v>
       </c>
       <c r="XT1340" s="14" t="str">
@@ -935,7 +1107,7 @@
         <v>655,1339</v>
       </c>
     </row>
-    <row r="1341" spans="636:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1341" spans="631:656" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="XP1341" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>639,1340</v>
@@ -945,11 +1117,11 @@
         <v>640,1340</v>
       </c>
       <c r="XR1341" s="5" t="str">
-        <f t="shared" ref="XR1341" ca="1" si="6">CONCATENATE(CELL("col",XR1341)-1,",",CELL("row",XR1341)-1)</f>
+        <f t="shared" ref="XR1341" ca="1" si="10">CONCATENATE(CELL("col",XR1341)-1,",",CELL("row",XR1341)-1)</f>
         <v>641,1340</v>
       </c>
       <c r="XS1341" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="9"/>
         <v>642,1340</v>
       </c>
       <c r="XT1341" s="15" t="str">

</xml_diff>